<commit_message>
I added an explanation to the excel visualisation in the newinsert branch
</commit_message>
<xml_diff>
--- a/Excel Visualization.xlsx
+++ b/Excel Visualization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moved Files\Desktop\Git Projects\Enterprise-Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C92D9DA-0274-468F-9A0B-0B302E7EEBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2052BB-8D64-4D59-AEE5-741EA1D7B15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{261B927B-A5D9-4B20-B651-222A144F1184}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261B927B-A5D9-4B20-B651-222A144F1184}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Revenue" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>EmployeeName</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Lionel Tapessi</t>
+  </si>
+  <si>
+    <t>Revenue generated per employee sales</t>
   </si>
 </sst>
 </file>
@@ -195,12 +198,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -215,8 +224,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3001,9 +3014,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3041,7 +3054,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3147,7 +3160,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3289,7 +3302,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3297,10 +3310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406CDF22-6DEC-4371-A278-1B3BE4AEF88D}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3312,7 +3325,7 @@
     <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3329,7 +3342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3346,7 +3359,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3363,7 +3376,7 @@
         <v>1150</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3380,7 +3393,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3397,7 +3410,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3414,7 +3427,19 @@
         <v>630</v>
       </c>
     </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="G10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G10:J10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3577,7 +3602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94873B68-415F-4C7F-8F0A-CBA54939E608}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
I removed unnecessry line of code explanations in sql file as well as doing a few modifications to the excel visualization file
</commit_message>
<xml_diff>
--- a/Excel Visualization.xlsx
+++ b/Excel Visualization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moved Files\Desktop\Git Projects\Enterprise-Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2052BB-8D64-4D59-AEE5-741EA1D7B15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319F757E-F27D-4503-98F9-0423A8043673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{261B927B-A5D9-4B20-B651-222A144F1184}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{261B927B-A5D9-4B20-B651-222A144F1184}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Revenue" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>EmployeeName</t>
   </si>
@@ -180,16 +180,13 @@
   </si>
   <si>
     <t>Lionel Tapessi</t>
-  </si>
-  <si>
-    <t>Revenue generated per employee sales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,19 +194,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -224,12 +238,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -277,13 +299,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -305,7 +333,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sales Revenue'!$D$1</c:f>
+              <c:f>'Sales Revenue'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -315,18 +343,47 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Sales Revenue'!$A$2:$A$6</c:f>
+              <c:f>'Sales Revenue'!$B$3:$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -349,7 +406,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sales Revenue'!$D$2:$D$6</c:f>
+              <c:f>'Sales Revenue'!$E$3:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -385,8 +442,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="932661887"/>
         <c:axId val="932665247"/>
       </c:barChart>
@@ -403,11 +460,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -421,9 +478,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -452,9 +508,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -480,9 +536,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -510,17 +565,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -570,13 +636,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -598,7 +670,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Inventory Management'!$C$1</c:f>
+              <c:f>'Inventory Management'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -608,18 +680,47 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Inventory Management'!$B$2:$B$12</c:f>
+              <c:f>'Inventory Management'!$C$3:$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -660,7 +761,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Inventory Management'!$C$2:$C$12</c:f>
+              <c:f>'Inventory Management'!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -714,7 +815,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
         <c:axId val="932656127"/>
         <c:axId val="932652287"/>
       </c:barChart>
@@ -731,11 +833,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -749,9 +851,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -780,9 +881,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -808,9 +909,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -838,17 +938,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -898,13 +1009,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -926,7 +1043,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Customer Segmentation'!$D$1</c:f>
+              <c:f>'Customer Segmentation'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -936,18 +1053,47 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Customer Segmentation'!$A$2:$A$22</c:f>
+              <c:f>'Customer Segmentation'!$B$3:$B$23</c:f>
               <c:strCache>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
@@ -1018,7 +1164,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Customer Segmentation'!$D$2:$D$22</c:f>
+              <c:f>'Customer Segmentation'!$E$3:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1102,8 +1248,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
         <c:axId val="932669567"/>
         <c:axId val="932662367"/>
       </c:barChart>
@@ -1120,11 +1266,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1138,9 +1284,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1169,9 +1314,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1197,9 +1342,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1227,17 +1371,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1380,35 +1535,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1416,26 +1569,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1444,9 +1605,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1465,14 +1625,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1481,35 +1633,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1521,30 +1673,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1560,21 +1713,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1584,20 +1734,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1608,17 +1758,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1627,14 +1777,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1646,28 +1795,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1679,17 +1822,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1698,17 +1840,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1717,17 +1859,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1736,27 +1877,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1764,11 +1904,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1776,14 +1926,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1795,12 +1945,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1809,14 +1966,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1825,9 +1981,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1837,7 +1992,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1845,9 +2000,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1858,9 +2013,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1870,48 +2024,40 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1919,26 +2065,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1947,9 +2101,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1968,14 +2121,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1984,20 +2129,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2006,13 +2151,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2024,10 +2169,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2036,16 +2181,17 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -2063,21 +2209,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2096,14 +2239,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2115,14 +2257,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2136,9 +2278,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2152,12 +2293,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -2169,9 +2304,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2186,14 +2321,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2205,14 +2339,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2224,14 +2358,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2240,14 +2373,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2255,7 +2387,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2268,11 +2400,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2280,14 +2422,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2299,12 +2441,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2320,7 +2469,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2329,9 +2477,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2347,14 +2494,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2363,9 +2509,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2377,46 +2522,38 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2424,26 +2561,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -2452,9 +2597,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2473,14 +2617,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2489,35 +2625,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2529,30 +2665,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2568,21 +2705,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2592,20 +2726,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2616,17 +2750,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2635,14 +2769,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2654,28 +2787,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2687,17 +2814,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2706,17 +2832,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2725,17 +2851,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2744,27 +2869,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2772,11 +2896,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2784,14 +2918,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2803,12 +2937,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2817,14 +2958,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2833,9 +2973,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2845,7 +2984,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2853,9 +2992,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2866,9 +3005,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2878,14 +3016,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2895,15 +3027,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>168275</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2935,16 +3067,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>225425</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>530225</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2976,15 +3108,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>492125</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>187325</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3310,136 +3442,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406CDF22-6DEC-4371-A278-1B3BE4AEF88D}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="C3" s="5">
         <v>299</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="E3" s="5">
         <v>36000</v>
       </c>
-      <c r="E2">
+      <c r="F3" s="5">
         <v>1855</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="C4" s="5">
         <v>300</v>
       </c>
-      <c r="C3">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E4" s="5">
         <v>22000</v>
       </c>
-      <c r="E3">
+      <c r="F4" s="5">
         <v>1150</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
+      <c r="C5" s="5">
         <v>297</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="E5" s="5">
         <v>15000</v>
       </c>
-      <c r="E4">
+      <c r="F5" s="5">
         <v>757</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="C6" s="5">
         <v>298</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="5">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="E6" s="5">
         <v>15000</v>
       </c>
-      <c r="E5">
+      <c r="F6" s="5">
         <v>757</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="C7" s="5">
         <v>294</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="E7" s="5">
         <v>12000</v>
       </c>
-      <c r="E6">
+      <c r="F7" s="5">
         <v>630</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="G10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G10:J10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3447,148 +3580,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53435224-F238-4133-BF86-2BF70D9E5940}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="7">
         <v>190</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="7">
         <v>191</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
+      <c r="D4" s="7">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="7">
         <v>192</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="7">
         <v>193</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="7">
         <v>194</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="7">
         <v>195</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C7">
+      <c r="D8" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="7">
         <v>196</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
+      <c r="D9" s="7">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="7">
         <v>197</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C9">
+      <c r="D10" s="7">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="7">
         <v>198</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C10">
+      <c r="D11" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="7">
         <v>199</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C11">
+      <c r="D12" s="7">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="7">
         <v>200</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12">
+      <c r="D13" s="7">
         <v>50</v>
       </c>
     </row>
@@ -3600,283 +3733,297 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94873B68-415F-4C7F-8F0A-CBA54939E608}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2">
+      <c r="C3" s="7">
         <v>112</v>
       </c>
-      <c r="C2">
+      <c r="D3" s="7">
         <v>11500</v>
       </c>
-      <c r="D2">
+      <c r="E3" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B3">
+      <c r="C4" s="7">
         <v>118</v>
       </c>
-      <c r="D3">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B4">
+      <c r="C5" s="7">
         <v>102</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
+      <c r="C6" s="7">
         <v>104</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B6">
+      <c r="C7" s="7">
         <v>105</v>
       </c>
-      <c r="C6">
+      <c r="D7" s="7">
         <v>15150</v>
       </c>
-      <c r="D6">
+      <c r="E7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7">
+      <c r="C8" s="7">
         <v>106</v>
       </c>
-      <c r="D7">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8">
+      <c r="C9" s="7">
         <v>107</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B9">
+      <c r="C10" s="7">
         <v>108</v>
       </c>
-      <c r="D9">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B10">
+      <c r="C11" s="7">
         <v>109</v>
       </c>
-      <c r="C10">
+      <c r="D11" s="7">
         <v>12600</v>
       </c>
-      <c r="D10">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B11">
+      <c r="C12" s="7">
         <v>110</v>
       </c>
-      <c r="D11">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B12">
+      <c r="C13" s="7">
         <v>111</v>
       </c>
-      <c r="D12">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B13">
+      <c r="C14" s="7">
         <v>119</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B14">
+      <c r="C15" s="7">
         <v>120</v>
       </c>
-      <c r="C14">
+      <c r="D15" s="7">
         <v>12600</v>
       </c>
-      <c r="D14">
+      <c r="E15" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B15">
+      <c r="C16" s="7">
         <v>121</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B16">
+      <c r="C17" s="7">
         <v>122</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="7"/>
+      <c r="E17" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B17">
+      <c r="C18" s="7">
         <v>123</v>
       </c>
-      <c r="C17">
+      <c r="D18" s="7">
         <v>24500</v>
       </c>
-      <c r="D17">
+      <c r="E18" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B18">
+      <c r="C19" s="7">
         <v>125</v>
       </c>
-      <c r="D18">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B19">
+      <c r="C20" s="7">
         <v>115</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B20">
+      <c r="C21" s="7">
         <v>116</v>
       </c>
-      <c r="C20">
+      <c r="D21" s="7">
         <v>15150</v>
       </c>
-      <c r="D20">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B21">
+      <c r="C22" s="7">
         <v>100</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B22">
+      <c r="C23" s="7">
         <v>101</v>
       </c>
-      <c r="C22">
+      <c r="D23" s="7">
         <v>11500</v>
       </c>
-      <c r="D22">
+      <c r="E23" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>